<commit_message>
Added frequency modification to dyspnea and updated the model to effect the target ventilation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dyspnea_update\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27555881-198A-40F6-BB1E-B04399C13B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316F1E7B-8667-43E2-846F-5D39022EC7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" tabRatio="643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8985" yWindow="1935" windowWidth="24135" windowHeight="21030" tabRatio="643" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2172" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="334">
   <si>
     <t>Oxygen Saturation</t>
   </si>
@@ -659,21 +659,9 @@
     <t>Right and left mainstem intubation and correction (with Succs)</t>
   </si>
   <si>
-    <t>Mild</t>
-  </si>
-  <si>
     <t>Healthy</t>
   </si>
   <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>Severe</t>
-  </si>
-  <si>
-    <t>Decrease to 0</t>
-  </si>
-  <si>
     <t>Decrease to ~70% of healthy</t>
   </si>
   <si>
@@ -773,18 +761,9 @@
     <t>Increase,  Tachypnea,   &gt; 30 @cite gunning2003pathophysiology</t>
   </si>
   <si>
-    <t>Dysnea: Severity = 0.3</t>
-  </si>
-  <si>
     <t>Dysnea: Severity = 0.0</t>
   </si>
   <si>
-    <t>Dysnea: Severity = 0.6</t>
-  </si>
-  <si>
-    <t>Dysnea: Severity = 1.0</t>
-  </si>
-  <si>
     <t>Dyspnea</t>
   </si>
   <si>
@@ -1020,6 +999,63 @@
   </si>
   <si>
     <t>0, Dyspnea</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volulme Severity = 0.3</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volulme Severity = 0.6</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volulme Severity = 1.0</t>
+  </si>
+  <si>
+    <t>Return to Normal</t>
+  </si>
+  <si>
+    <t>Dysnea: Respiration Rate Severity = 0.3</t>
+  </si>
+  <si>
+    <t>Dysnea: Respiration Rate Severity = 0.6</t>
+  </si>
+  <si>
+    <t>Dysnea: Respiration Rate Severity = 1.0</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volume Severity = 0.3, Respiration Rate Severity = 0.3</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volume Severity = 0.6, Respiration Rate Severity = 0.6</t>
+  </si>
+  <si>
+    <t>Dysnea: Tidal Volume Severity = 1.0, Respiration Rate Severity = 1.0</t>
+  </si>
+  <si>
+    <t>Mild amplitude effect</t>
+  </si>
+  <si>
+    <t>Moderate amplitude effect</t>
+  </si>
+  <si>
+    <t>Full amplitude effect</t>
+  </si>
+  <si>
+    <t>Mild frequency effect</t>
+  </si>
+  <si>
+    <t>Moderate frequency effect</t>
+  </si>
+  <si>
+    <t>Full frequency effect</t>
+  </si>
+  <si>
+    <t>Mild amplitude and frequency effect</t>
+  </si>
+  <si>
+    <t>Moderate amplitude and frequency effect</t>
+  </si>
+  <si>
+    <t>Full amplitude and frequency effect</t>
   </si>
 </sst>
 </file>
@@ -2139,8 +2175,8 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2310,7 +2346,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>98</v>
@@ -2409,13 +2445,13 @@
         <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>98</v>
@@ -2444,7 +2480,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
@@ -2479,7 +2515,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>46</v>
@@ -2514,7 +2550,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>46</v>
@@ -2549,13 +2585,13 @@
         <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>98</v>
@@ -2654,13 +2690,13 @@
         <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>98</v>
@@ -2829,7 +2865,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>46</v>
@@ -2841,7 +2877,7 @@
         <v>98</v>
       </c>
       <c r="F20" s="20">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>101</v>
@@ -2864,13 +2900,13 @@
         <v>46</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>98</v>
@@ -2910,7 +2946,7 @@
       </c>
       <c r="F22" s="20">
         <f>SUM(F3:F21)</f>
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>101</v>
@@ -2992,7 +3028,7 @@
         <v>46</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -3119,7 +3155,7 @@
         <v>180</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>163</v>
@@ -3358,7 +3394,7 @@
         <v>98</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>100</v>
@@ -3512,7 +3548,7 @@
         <v>46</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -3736,7 +3772,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>46</v>
@@ -3911,7 +3947,7 @@
         <v>46</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -4023,7 +4059,7 @@
         <v>46</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>46</v>
@@ -4142,28 +4178,30 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -4180,7 +4218,7 @@
         <v>46</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -4197,8 +4235,14 @@
       <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>46</v>
       </c>
@@ -4232,19 +4276,25 @@
       <c r="K2" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="L2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>239</v>
+        <v>315</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>201</v>
+        <v>325</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>46</v>
@@ -4262,184 +4312,425 @@
         <v>98</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>240</v>
+        <v>316</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>202</v>
+        <v>326</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F4" s="5">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="5">
         <v>210</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="5">
-        <v>510</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>26</v>
+        <v>203</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>241</v>
+        <v>317</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>203</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="5">
-        <v>510</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="5">
-        <v>690</v>
+        <v>210</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J5" s="7" t="s">
-        <v>207</v>
+      <c r="J5" s="7">
+        <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F6" s="5">
-        <v>690</v>
+        <v>210</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="5">
-        <v>990</v>
+        <v>510</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>26</v>
+        <v>318</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>242</v>
+        <v>319</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="5">
-        <v>990</v>
+        <v>30</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="5">
-        <v>1170</v>
+        <v>210</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>205</v>
+      <c r="J7" s="6" t="s">
+        <v>303</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>202</v>
+        <v>329</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F8" s="5">
-        <v>1170</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="H8" s="5">
-        <v>1650</v>
+        <v>210</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>26</v>
+      <c r="J8" s="6" t="s">
+        <v>303</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="5">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="5">
+        <v>210</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="5">
+        <v>210</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="5">
+        <v>510</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5">
+        <v>30</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="5">
+        <v>210</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="5">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="5">
+        <v>210</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="5">
+        <v>30</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="5">
+        <v>210</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="7">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4473,7 +4764,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4493,7 +4784,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -4505,7 +4796,7 @@
         <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>46</v>
@@ -4551,13 +4842,13 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -4575,7 +4866,7 @@
         <v>98</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>99</v>
@@ -4583,7 +4874,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4603,7 +4894,7 @@
         <v>46</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>46</v>
@@ -4615,7 +4906,7 @@
         <v>46</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>46</v>
@@ -4661,13 +4952,13 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>46</v>
@@ -4685,7 +4976,7 @@
         <v>98</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>99</v>
@@ -4693,7 +4984,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4725,7 +5016,7 @@
         <v>46</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>46</v>
@@ -4771,13 +5062,13 @@
         <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>46</v>
@@ -4795,7 +5086,7 @@
         <v>98</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>99</v>
@@ -4871,7 +5162,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -5204,7 +5495,7 @@
         <v>46</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>46</v>
@@ -6117,7 +6408,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
@@ -6141,7 +6432,7 @@
         <v>101</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>101</v>
@@ -6357,7 +6648,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
@@ -6507,7 +6798,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6542,7 +6833,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="V1" s="12"/>
     </row>
@@ -6569,7 +6860,7 @@
         <v>46</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>46</v>
@@ -6581,7 +6872,7 @@
         <v>46</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>46</v>
@@ -6593,7 +6884,7 @@
         <v>46</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>46</v>
@@ -6617,7 +6908,7 @@
         <v>46</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>46</v>
@@ -6705,13 +6996,13 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -6723,55 +7014,55 @@
         <v>98</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="O4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="S4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>99</v>
@@ -6870,7 +7161,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -7032,7 +7323,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
@@ -7050,7 +7341,7 @@
         <v>101</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>100</v>
@@ -7109,7 +7400,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -7271,7 +7562,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
@@ -7345,7 +7636,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -7507,7 +7798,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>46</v>
@@ -7687,7 +7978,7 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
@@ -7849,13 +8140,13 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -7867,19 +8158,19 @@
         <v>98</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="J4" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>238</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>245</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>100</v>
@@ -7891,31 +8182,31 @@
         <v>102</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="X4" s="14" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>99</v>
@@ -7986,7 +8277,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -8040,7 +8331,7 @@
         <v>46</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>46</v>
@@ -8128,13 +8419,13 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -8205,7 +8496,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>46</v>
@@ -8271,7 +8562,7 @@
         <v>100</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="Y5" s="2" t="s">
         <v>99</v>
@@ -8282,7 +8573,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
@@ -8348,7 +8639,7 @@
         <v>100</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="Y6" s="2" t="s">
         <v>99</v>
@@ -8359,7 +8650,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>46</v>
@@ -8425,7 +8716,7 @@
         <v>100</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="Y7" s="2" t="s">
         <v>99</v>
@@ -8579,7 +8870,7 @@
         <v>100</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Y9" s="2" t="s">
         <v>99</v>
@@ -8749,7 +9040,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>46</v>
@@ -8826,7 +9117,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>46</v>
@@ -8892,7 +9183,7 @@
         <v>100</v>
       </c>
       <c r="X15" s="6" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="Y15" s="2" t="s">
         <v>99</v>
@@ -8903,7 +9194,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>46</v>
@@ -8969,7 +9260,7 @@
         <v>100</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="Y16" s="2" t="s">
         <v>99</v>
@@ -8980,7 +9271,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>46</v>
@@ -9046,7 +9337,7 @@
         <v>100</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="Y17" s="2" t="s">
         <v>99</v>
@@ -9123,7 +9414,7 @@
         <v>100</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Y18" s="2" t="s">
         <v>99</v>
@@ -9159,7 +9450,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="60" x14ac:dyDescent="0.25">
@@ -9179,7 +9470,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>46</v>
@@ -9191,13 +9482,13 @@
         <v>46</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>46</v>
@@ -9221,7 +9512,7 @@
         <v>46</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>46</v>
@@ -9309,13 +9600,13 @@
         <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>46</v>
@@ -9380,13 +9671,13 @@
         <v>46</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>46</v>
@@ -9404,43 +9695,43 @@
         <v>98</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>101</v>
       </c>
       <c r="R5" s="13" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="S5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>101</v>
       </c>
       <c r="V5" s="13" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>99</v>
@@ -9451,13 +9742,13 @@
         <v>46</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>46</v>
@@ -9475,43 +9766,43 @@
         <v>98</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>101</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>99</v>
@@ -9522,13 +9813,13 @@
         <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>46</v>
@@ -9546,43 +9837,43 @@
         <v>98</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="S7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>99</v>
@@ -9593,13 +9884,13 @@
         <v>46</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>46</v>
@@ -9617,43 +9908,43 @@
         <v>98</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>99</v>
@@ -9664,13 +9955,13 @@
         <v>46</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>46</v>
@@ -9688,43 +9979,43 @@
         <v>98</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="W9" s="2" t="s">
         <v>99</v>
@@ -9787,7 +10078,7 @@
         <v>46</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>46</v>
@@ -10153,7 +10444,7 @@
         <v>98</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>100</v>

</xml_diff>